<commit_message>
added to be 18 date added resource images onscreen keyboard works fine adjusted theming for keyboard screens
</commit_message>
<xml_diff>
--- a/Resources/XLSX/StaffID.xlsx
+++ b/Resources/XLSX/StaffID.xlsx
@@ -56,9 +56,6 @@
   </x:si>
   <x:si>
     <x:t>NATHAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TEST</x:t>
   </x:si>
   <x:si>
     <x:t>2222</x:t>
@@ -419,7 +416,7 @@
   <x:dimension ref="A1:D4"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="E6" sqref="E6 E4 E5"/>
+      <x:selection activeCell="E6" sqref="E6 E3 E4 E5"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,10 +474,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
         <x:v>11</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>12</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>4</x:v>

</xml_diff>

<commit_message>
panel themes fixed. dont like the code. but it works. now to work on images
</commit_message>
<xml_diff>
--- a/Resources/XLSX/StaffID.xlsx
+++ b/Resources/XLSX/StaffID.xlsx
@@ -43,22 +43,22 @@
     <x:t>1111</x:t>
   </x:si>
   <x:si>
+    <x:t>NATHAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DANSKIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2222</x:t>
+  </x:si>
+  <x:si>
     <x:t>ALANA</x:t>
   </x:si>
   <x:si>
-    <x:t>DANSKIN</x:t>
-  </x:si>
-  <x:si>
     <x:t>3333</x:t>
   </x:si>
   <x:si>
     <x:t>MANAGER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NATHAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2222</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -466,21 +466,21 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
         <x:v>11</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Massive theming update need to add in the theming change panel to start coding variables for theme changing
</commit_message>
<xml_diff>
--- a/Resources/XLSX/StaffID.xlsx
+++ b/Resources/XLSX/StaffID.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DA8D8E-5B1E-4244-BE1F-5C3DCB185367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30045207-B7B2-4CC1-95CB-7D010F0AB0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -416,7 +416,7 @@
   <x:dimension ref="A1:D4"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="E6" sqref="E6 E3 E4 E5"/>
+      <x:selection activeCell="A7" sqref="A7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +455,7 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4">
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -469,7 +469,7 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A4" s="0" t="s">
         <x:v>9</x:v>
       </x:c>

</xml_diff>